<commit_message>
feat: add new table m user selected
</commit_message>
<xml_diff>
--- a/excel/m_thread_data.xlsx
+++ b/excel/m_thread_data.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DEV\FLUTTER\project\MY_GITHUB\thread_fon\thread_fon_db\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{342E3ABC-96A9-4277-951E-8F72FCF4941C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2027BD9-E336-4961-8C35-F34653E24BE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{065E2E10-44EF-4F04-9A81-3EF8E78F7D6E}"/>
+    <workbookView xWindow="3840" yWindow="2280" windowWidth="18000" windowHeight="9810" activeTab="3" xr2:uid="{065E2E10-44EF-4F04-9A81-3EF8E78F7D6E}"/>
   </bookViews>
   <sheets>
     <sheet name="m_tolerance" sheetId="4" r:id="rId1"/>
     <sheet name="m_profile" sheetId="2" r:id="rId2"/>
     <sheet name="m_diam_pitch_range_dimension" sheetId="3" r:id="rId3"/>
+    <sheet name="m_user_selected" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="170">
   <si>
     <t>pitch</t>
   </si>
@@ -508,6 +509,45 @@
   <si>
     <t>d1_ei_8h_f</t>
   </si>
+  <si>
+    <t>range_1</t>
+  </si>
+  <si>
+    <t>range_2</t>
+  </si>
+  <si>
+    <t>range_3</t>
+  </si>
+  <si>
+    <t>coarse_pitch</t>
+  </si>
+  <si>
+    <t>1.25,1</t>
+  </si>
+  <si>
+    <t>tolerance</t>
+  </si>
+  <si>
+    <t>6H</t>
+  </si>
+  <si>
+    <t>6h</t>
+  </si>
+  <si>
+    <t>7h5g</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>fine_pitch</t>
+  </si>
+  <si>
+    <t>extra_fine_pitch</t>
+  </si>
 </sst>
 </file>
 
@@ -886,7 +926,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F3E1EE5-36CA-4568-AA50-5AD4E0DC26A6}">
   <dimension ref="A1:EO69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="DM1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="DU6" sqref="DU6"/>
     </sheetView>
   </sheetViews>
@@ -54788,4 +54828,111 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{067C2734-791D-485E-BD73-996B5BA40D2F}">
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="14.85546875" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" customWidth="1"/>
+    <col min="8" max="8" width="19.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E1" t="s">
+        <v>159</v>
+      </c>
+      <c r="F1" t="s">
+        <v>160</v>
+      </c>
+      <c r="G1" t="s">
+        <v>168</v>
+      </c>
+      <c r="H1" t="s">
+        <v>169</v>
+      </c>
+      <c r="I1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F2">
+        <v>1.2</v>
+      </c>
+      <c r="H2" t="s">
+        <v>161</v>
+      </c>
+      <c r="I2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2.5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>166</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3" t="s">
+        <v>161</v>
+      </c>
+      <c r="I3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1.25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>166</v>
+      </c>
+      <c r="I4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>